<commit_message>
Update English manuals to v1.10.0
</commit_message>
<xml_diff>
--- a/asset/Documents/Exastro-ITA_[Reference]Configuration_settings_during_installation.xlsx
+++ b/asset/Documents/Exastro-ITA_[Reference]Configuration_settings_during_installation.xlsx
@@ -4,23 +4,26 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="6588"/>
   </bookViews>
   <sheets>
     <sheet name="1. MariaDB(server.cnf)" sheetId="2" r:id="rId1"/>
     <sheet name="2. PHP(php.ini)" sheetId="4" r:id="rId2"/>
     <sheet name="3. ansible.cfg" sheetId="3" r:id="rId3"/>
     <sheet name="4. ITA setting file description" sheetId="9" r:id="rId4"/>
+    <sheet name="5．php-fpm(www.conf)" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. MariaDB(server.cnf)'!$B$9:$H$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. PHP(php.ini)'!$B$9:$H$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'3. ansible.cfg'!$B$5:$G$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4. ITA setting file description'!$B$6:$K$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'5．php-fpm(www.conf)'!$B$10:$H$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'1. MariaDB(server.cnf)'!$A$2:$H$23</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'2. PHP(php.ini)'!$A$2:$H$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'2. PHP(php.ini)'!$A$2:$H$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'3. ansible.cfg'!$A$2:$G$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'4. ITA setting file description'!$A$1:$J$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'5．php-fpm(www.conf)'!$A$1:$H$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2. PHP(php.ini)'!$2:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'3. ansible.cfg'!$2:$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'4. ITA setting file description'!$1:$6</definedName>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="262">
   <si>
     <t>№</t>
     <phoneticPr fontId="1"/>
@@ -49,14 +52,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>OpenStack</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DSC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>№</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -123,10 +118,6 @@
   </si>
   <si>
     <t>○</t>
-  </si>
-  <si>
-    <t>AnsibleTower</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>OFF</t>
@@ -191,10 +182,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Consider tuning depending on how to use ITA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Required/
 For reference</t>
     <phoneticPr fontId="1"/>
@@ -225,46 +212,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Consider tuning depending on how to use ITA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Modify the setting to hide PHP version
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Consider the tuning if timeout occurs when using ITA
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Consider the tuning if timeout occurs when using ITA
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Consider the tuning if memory allocation is not enough for PHP when using ITA
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Consider the tuning if large capacity registered/updated can't be performed when using ITA 
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Consider the tuning according to the file size that users want to upload in ITA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ITA uses PHP with PDO to connect to MySQL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The directory mentioned in the modification is required to be created in advance.
-The default directory(/tmp) is not recommended
-</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -276,11 +224,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Control garbage collection of PHP session file. 
-According to the setting on the left with the combination of the default value session.gc_probability = 1, the session file that passed 12 hours or more is in 100% probability to be performed garbage collection.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Setting file name</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -290,6 +233,12 @@
   </si>
   <si>
     <t>Define the root path of data relay storage in Cobbler server</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The execution time limit of data portability import process. 
+The process during execution will be determined as failed if the execution time passed the setting value.
+The unit is second.Default value is 300</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -431,6 +380,9 @@
   </si>
   <si>
     <t>(ITA installed directory)/ita-root/confs/restapiconfs/ansible_driver/ansible_playbook_watch_time.txt</t>
+  </si>
+  <si>
+    <t>(ITA installed directory)/ita-root/confs/commonconfs/admin_mail_addr.txt</t>
   </si>
   <si>
     <t>(ITA installed directory)/ita-root/confs/webconfs/ExternalAuthSettings.ini</t>
@@ -650,9 +602,6 @@
     <t>pdo_mysql.default_socket</t>
   </si>
   <si>
-    <t>（値空白）</t>
-  </si>
-  <si>
     <t>/var/lib/mysql/mysql.sock</t>
   </si>
   <si>
@@ -737,10 +686,6 @@
     <t>yaml.so</t>
   </si>
   <si>
-    <t>（No such value）</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Setting item</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -899,13 +844,132 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>The execution time limit of data portability import process. 
-The process during execution will be determined as failed if the execution time passed the setting value.
-The unit is second.Default value is 18000</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>(ITA installed directory)/ita-root/confs/webconfs/admin_mail_addr.txt</t>
+    <t>Tune to fit your ITA Environment if necessary</t>
+  </si>
+  <si>
+    <t>Change if you want to hide the PHP version.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify if timeout occurs when using ITA
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify if the current memory allocation is not enough for PHP when using ITA
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify if large capacity register/update operations can't be performed when using ITA 
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Modify according to the file size that users want to upload in ITA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The directory mentioned in the modification must be created in advance.
+It is not recommended that the user use the default directory, (/tmp).
+※Uncomment + Modify
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Control garbage collection of PHP session file. 
+According to the setting on the left Controls the PHP Session file GC (garbage collection).
+According to the settings on the left
+ (Combination of session.gc_probability = 1 and default values)
+ any session files that exceeds 12 hours will be put in to the GC with a 100% probability.with the combination of the default value session.gc_probability = 1, the session file that passed 12 hours or more is in 100% probability to be performed garbage collection.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>session.cookie_httponly</t>
+  </si>
+  <si>
+    <t>(No value)</t>
+  </si>
+  <si>
+    <t>(No value)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※Add</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（Blank）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>php_admin_value[memory_limit]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>128M</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2048M</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>php_value[session.save_path]</t>
+  </si>
+  <si>
+    <t>/var/lib/php/session</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ansible Tower</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Terraform</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CI/CD For IaC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5．php-fpm(www.conf) setting value modification list.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deployed if running on RHEL8 type server.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The following settings are set to run on an ITA System server with the minimum required specs. (CPU: Duo core / Memory: 4GB) 。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The tuning values are catered to an ITA System server with the following specs: (CPU: Quad core / Memory: 8GB)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※1  ITA system server = Basic ITA Configuration where Ansible servers and other driver servers are constructed seperately.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tuning value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Reference</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(ITA install directory)/ita_sessions</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Change</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -913,7 +977,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1032,6 +1096,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="メイリオ"/>
       <family val="3"/>
@@ -1174,7 +1245,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1340,8 +1411,59 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1653,77 +1775,77 @@
   </sheetPr>
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="1.6640625" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="17"/>
+    <col min="1" max="1" width="1.6640625" style="17"/>
     <col min="2" max="2" width="4" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="27.875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.5" style="17" customWidth="1"/>
-    <col min="8" max="8" width="60.625" style="17" customWidth="1"/>
-    <col min="9" max="16384" width="1.625" style="17"/>
+    <col min="3" max="3" width="15.33203125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.44140625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="60.6640625" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="1.6640625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="3" customHeight="1"/>
-    <row r="2" spans="1:8" ht="45.95" customHeight="1">
+    <row r="2" spans="1:8" ht="45.9" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="22.5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21.6">
       <c r="B3" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="22.5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21.6">
       <c r="B5" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="22.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21.6">
       <c r="B6" s="19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="22.5">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21.6">
       <c r="B7" s="15" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="6" customHeight="1">
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:8" ht="33">
+    <row r="9" spans="1:8" ht="32.4">
       <c r="B9" s="24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1">
@@ -1731,13 +1853,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="30" t="b">
         <v>1</v>
@@ -1752,19 +1874,19 @@
         <v>2</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="H11" s="31"/>
     </row>
@@ -1773,22 +1895,22 @@
         <v>3</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1796,22 +1918,22 @@
         <v>4</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="H13" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1">
@@ -1819,22 +1941,22 @@
         <v>5</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1">
@@ -1842,22 +1964,22 @@
         <v>6</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1">
@@ -1865,10 +1987,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E16" s="36">
         <v>0</v>
@@ -1880,7 +2002,7 @@
         <v>100</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="30" customHeight="1">
@@ -1888,22 +2010,22 @@
         <v>8</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G17" s="38" t="s">
-        <v>137</v>
-      </c>
       <c r="H17" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1">
@@ -1911,22 +2033,22 @@
         <v>9</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F18" s="40" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H18" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="30" customHeight="1">
@@ -1934,13 +2056,13 @@
         <v>10</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F19" s="40">
         <v>1</v>
@@ -1955,22 +2077,22 @@
         <v>11</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H20" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="30" customHeight="1">
@@ -1978,22 +2100,22 @@
         <v>12</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="30" customHeight="1">
@@ -2001,22 +2123,22 @@
         <v>13</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H22" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -2024,10 +2146,10 @@
         <v>14</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E23" s="36">
         <v>151</v>
@@ -2039,7 +2161,7 @@
         <v>5000</v>
       </c>
       <c r="H23" s="39" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="10:11">
@@ -2118,78 +2240,78 @@
     <tabColor rgb="FFCC9900"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="1.6640625" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="17"/>
+    <col min="1" max="1" width="1.6640625" style="17"/>
     <col min="2" max="2" width="4" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="35.25" style="17" customWidth="1"/>
-    <col min="5" max="5" width="45.625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="55.625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="60.625" style="17" customWidth="1"/>
-    <col min="9" max="16384" width="1.625" style="17"/>
+    <col min="3" max="3" width="12.88671875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="35.21875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="55.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.6640625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="60.6640625" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="1.6640625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="3" customHeight="1"/>
-    <row r="2" spans="1:8" ht="35.25">
+    <row r="2" spans="1:8" ht="34.799999999999997">
       <c r="A2" s="16" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B2" s="15"/>
     </row>
-    <row r="3" spans="1:8" ht="36.950000000000003" customHeight="1">
+    <row r="3" spans="1:8" ht="36.9" customHeight="1">
       <c r="B3" s="42" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="11.1" customHeight="1"/>
-    <row r="5" spans="1:8" ht="18.95" customHeight="1">
+    <row r="5" spans="1:8" ht="18.899999999999999" customHeight="1">
       <c r="B5" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.95" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.899999999999999" customHeight="1">
       <c r="B6" s="19" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1">
       <c r="B7" s="15" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="5.0999999999999996" customHeight="1"/>
-    <row r="9" spans="1:8" ht="33">
+    <row r="9" spans="1:8" ht="48.6">
       <c r="B9" s="24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>46</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
@@ -2197,10 +2319,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E10" s="37">
         <v>4096</v>
@@ -2212,7 +2334,7 @@
         <v>16384</v>
       </c>
       <c r="H10" s="39" t="s">
-        <v>51</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
@@ -2220,22 +2342,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="H11" s="39" t="s">
-        <v>52</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1">
@@ -2243,10 +2365,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E12" s="37">
         <v>30</v>
@@ -2258,7 +2380,7 @@
         <v>600</v>
       </c>
       <c r="H12" s="39" t="s">
-        <v>53</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
@@ -2266,10 +2388,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E13" s="37">
         <v>60</v>
@@ -2281,7 +2403,7 @@
         <v>600</v>
       </c>
       <c r="H13" s="39" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" customHeight="1">
@@ -2289,22 +2411,22 @@
         <v>5</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>55</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" customHeight="1">
@@ -2312,22 +2434,22 @@
         <v>6</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>56</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" customHeight="1">
@@ -2335,22 +2457,22 @@
         <v>7</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>57</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="45" customHeight="1">
@@ -2358,10 +2480,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E17" s="37">
         <v>60</v>
@@ -2373,7 +2495,7 @@
         <v>600</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>51</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="45" customHeight="1">
@@ -2381,19 +2503,19 @@
         <v>9</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" s="47" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H18" s="48"/>
     </row>
@@ -2402,10 +2524,10 @@
         <v>10</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E19" s="37">
         <v>2000</v>
@@ -2417,7 +2539,7 @@
         <v>8000</v>
       </c>
       <c r="H19" s="39" t="s">
-        <v>51</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="45" customHeight="1">
@@ -2425,22 +2547,22 @@
         <v>11</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D20" s="47" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>163</v>
+        <v>243</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="J20" s="18"/>
     </row>
@@ -2449,10 +2571,10 @@
         <v>12</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E21" s="37">
         <v>2000</v>
@@ -2464,7 +2586,7 @@
         <v>8000</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>51</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="45" customHeight="1">
@@ -2472,10 +2594,10 @@
         <v>13</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E22" s="37">
         <v>60</v>
@@ -2487,7 +2609,7 @@
         <v>600</v>
       </c>
       <c r="H22" s="39" t="s">
-        <v>51</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="66" customHeight="1">
@@ -2495,22 +2617,22 @@
         <v>14</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="H23" s="31" t="s">
-        <v>59</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="45" customHeight="1">
@@ -2518,10 +2640,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D24" s="47" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E24" s="30">
         <v>1000</v>
@@ -2532,8 +2654,8 @@
       <c r="G24" s="30">
         <v>1</v>
       </c>
-      <c r="H24" s="56" t="s">
-        <v>62</v>
+      <c r="H24" s="73" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="45" customHeight="1">
@@ -2541,10 +2663,10 @@
         <v>16</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D25" s="47" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E25" s="30">
         <v>1440</v>
@@ -2555,29 +2677,29 @@
       <c r="G25" s="30">
         <v>43200</v>
       </c>
-      <c r="H25" s="56"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="2:10" ht="45" customHeight="1">
       <c r="B26" s="26">
         <v>17</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D26" s="47" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H26" s="49" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="45" customHeight="1">
@@ -2585,22 +2707,22 @@
         <v>18</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D27" s="47" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="H27" s="49" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="J27" s="18"/>
     </row>
@@ -2609,22 +2731,22 @@
         <v>19</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D28" s="47" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="H28" s="49" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="J28" s="18"/>
     </row>
@@ -2633,22 +2755,22 @@
         <v>20</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D29" s="47" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="H29" s="49" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="45" customHeight="1">
@@ -2656,22 +2778,22 @@
         <v>21</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D30" s="47" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="H30" s="49" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="45" customHeight="1">
@@ -2679,22 +2801,22 @@
         <v>22</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="H31" s="49" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="45" customHeight="1">
@@ -2702,48 +2824,71 @@
         <v>23</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="H32" s="49" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="45" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" s="53" customFormat="1" ht="45" customHeight="1">
       <c r="B33" s="26">
         <v>24</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D33" s="47" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E33" s="50" t="s">
-        <v>192</v>
+        <v>240</v>
       </c>
       <c r="F33" s="50" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="G33" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="H33" s="49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="45" customHeight="1"/>
+        <v>179</v>
+      </c>
+      <c r="H33" s="55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="45" customHeight="1">
+      <c r="B34" s="26">
+        <v>25</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="E34" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="F34" s="50">
+        <v>1</v>
+      </c>
+      <c r="G34" s="50">
+        <v>1</v>
+      </c>
+      <c r="H34" s="48" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="45" customHeight="1"/>
   </sheetData>
   <autoFilter ref="B9:H32"/>
   <mergeCells count="1">
@@ -2767,23 +2912,23 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="1.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" customWidth="1"/>
-    <col min="4" max="4" width="25.625" style="46" customWidth="1"/>
-    <col min="5" max="5" width="55.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="108.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="108.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="3" customHeight="1"/>
-    <row r="2" spans="1:9" ht="25.5">
+    <row r="2" spans="1:9" ht="25.8">
       <c r="A2" s="8" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
@@ -2792,9 +2937,9 @@
       <c r="F2" s="53"/>
       <c r="G2" s="53"/>
     </row>
-    <row r="3" spans="1:9" ht="22.5">
+    <row r="3" spans="1:9" ht="21.6">
       <c r="B3" s="15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C3" s="53"/>
       <c r="D3" s="53"/>
@@ -2810,24 +2955,24 @@
       <c r="F4" s="53"/>
       <c r="G4" s="53"/>
     </row>
-    <row r="5" spans="1:9" ht="56.25">
+    <row r="5" spans="1:9" ht="52.2">
       <c r="B5" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1">
@@ -2835,19 +2980,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G6" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1">
@@ -2855,19 +3000,19 @@
         <v>2</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G7" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1">
@@ -2875,19 +3020,19 @@
         <v>3</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="51">
         <v>5</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1">
@@ -2895,19 +3040,19 @@
         <v>4</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="51">
         <v>15</v>
       </c>
       <c r="G9" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1">
@@ -2915,19 +3060,19 @@
         <v>5</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1">
@@ -2935,19 +3080,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="G11" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -2956,19 +3101,19 @@
         <v>7</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="G12" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1">
@@ -2976,19 +3121,19 @@
         <v>8</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="G13" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1">
@@ -2996,19 +3141,19 @@
         <v>9</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="F14" s="51" t="b">
         <v>0</v>
       </c>
       <c r="G14" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1">
@@ -3016,19 +3161,19 @@
         <v>10</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="G15" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -3037,19 +3182,19 @@
         <v>11</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F16" s="51">
         <v>60</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -3058,19 +3203,19 @@
         <v>12</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="G17" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1">
@@ -3078,19 +3223,19 @@
         <v>13</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="F18" s="51" t="b">
         <v>0</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1">
@@ -3098,19 +3243,19 @@
         <v>14</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1">
@@ -3118,19 +3263,19 @@
         <v>15</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="G20" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1">
@@ -3138,19 +3283,19 @@
         <v>16</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G21" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1">
@@ -3158,19 +3303,19 @@
         <v>17</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="G22" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1">
@@ -3178,19 +3323,19 @@
         <v>18</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1">
@@ -3198,19 +3343,19 @@
         <v>19</v>
       </c>
       <c r="C24" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="G24" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1">
@@ -3218,19 +3363,19 @@
         <v>20</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F25" s="51" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1">
@@ -3238,19 +3383,19 @@
         <v>21</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="E26" s="52" t="s">
-        <v>236</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>243</v>
+        <v>223</v>
+      </c>
+      <c r="F26" s="56" t="s">
+        <v>230</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1">
@@ -3258,19 +3403,19 @@
         <v>22</v>
       </c>
       <c r="C27" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="E27" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="55">
+        <v>7</v>
+      </c>
+      <c r="F27" s="56">
         <v>5099</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1">
@@ -3278,19 +3423,19 @@
         <v>23</v>
       </c>
       <c r="C28" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E28" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="55">
+        <v>6</v>
+      </c>
+      <c r="F28" s="56">
         <v>30</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1">
@@ -3298,19 +3443,19 @@
         <v>24</v>
       </c>
       <c r="C29" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E29" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="55">
         <v>5</v>
       </c>
+      <c r="F29" s="56">
+        <v>5</v>
+      </c>
       <c r="G29" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1">
@@ -3318,19 +3463,19 @@
         <v>25</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="55">
+        <v>4</v>
+      </c>
+      <c r="F30" s="56">
         <v>30</v>
       </c>
       <c r="G30" s="54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="9:10">
@@ -3395,7 +3540,7 @@
   <autoFilter ref="B5:G27"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3407,73 +3552,73 @@
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="1.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="10.875" customWidth="1"/>
-    <col min="9" max="9" width="117.625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="76.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="117.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="76.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.5">
+    <row r="1" spans="1:11" ht="25.8">
       <c r="A1" s="8" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1"/>
-    <row r="3" spans="1:11" ht="17.25">
+    <row r="3" spans="1:11" ht="16.2">
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="57" t="s">
-        <v>64</v>
+      <c r="C5" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="58"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>4</v>
+        <v>251</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
+        <v>252</v>
+      </c>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
     </row>
     <row r="7" spans="1:11" ht="67.5" customHeight="1">
       <c r="B7" s="9">
@@ -3481,17 +3626,17 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="11" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="67.5" customHeight="1">
@@ -3499,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -3507,10 +3652,10 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="11" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>244</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="67.5" customHeight="1">
@@ -3518,24 +3663,24 @@
         <v>3</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="11" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="67.5" customHeight="1">
@@ -3543,28 +3688,28 @@
         <v>4</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="67.5" customHeight="1">
@@ -3572,28 +3717,28 @@
         <v>5</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="67.5" customHeight="1">
@@ -3601,7 +3746,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -3609,10 +3754,10 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="11" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="110.1" customHeight="1">
@@ -3621,19 +3766,19 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="H13" s="10"/>
       <c r="I13" s="11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="67.5" customHeight="1">
@@ -3641,7 +3786,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3649,10 +3794,10 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="11" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="K14" s="1"/>
     </row>
@@ -3661,24 +3806,28 @@
         <v>9</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="G15" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="67.5" customHeight="1">
@@ -3686,28 +3835,28 @@
         <v>10</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="67.5" customHeight="1">
@@ -3715,28 +3864,28 @@
         <v>11</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="K17" s="1"/>
     </row>
@@ -3745,28 +3894,28 @@
         <v>12</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="67.5" customHeight="1">
@@ -3774,28 +3923,28 @@
         <v>13</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="K19" s="1"/>
     </row>
@@ -3804,41 +3953,41 @@
         <v>14</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="H20" s="10"/>
       <c r="I20" s="11" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="52.8">
       <c r="B21" s="9">
         <v>15</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="11" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="67.5" customHeight="1">
@@ -3847,44 +3996,44 @@
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="54">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="52.8">
       <c r="B23" s="9">
         <v>17</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="11" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="54">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="52.8">
       <c r="B24" s="9">
         <v>18</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -3892,18 +4041,18 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="11" t="s">
-        <v>245</v>
+        <v>91</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="18.75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="17.399999999999999">
       <c r="B25" s="9">
         <v>19</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -3911,18 +4060,18 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="11" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" ht="27">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="26.4">
       <c r="B26" s="9">
         <v>20</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -3930,49 +4079,65 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="11" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="27">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="26.4">
       <c r="B27" s="9">
         <v>21</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I27" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="17.399999999999999">
+      <c r="C28" s="12"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" t="s">
         <v>105</v>
       </c>
-      <c r="J27" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11">
-      <c r="J28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11">
+    </row>
+    <row r="29" spans="2:11" ht="17.399999999999999">
+      <c r="C29" s="12"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="J29" s="14" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3987,4 +4152,205 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E24" sqref="E24"/>
+      <selection pane="topRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="1.6640625" defaultRowHeight="17.399999999999999"/>
+  <cols>
+    <col min="1" max="1" width="1.6640625" style="53"/>
+    <col min="2" max="2" width="4" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="53" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="28.77734375" style="53" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="63" customWidth="1"/>
+    <col min="8" max="8" width="61.88671875" style="53" customWidth="1"/>
+    <col min="9" max="16384" width="1.6640625" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24.75" customHeight="1">
+      <c r="A1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="60"/>
+    </row>
+    <row r="2" spans="1:8" ht="10.5" customHeight="1">
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="60"/>
+    </row>
+    <row r="3" spans="1:8" ht="21.6">
+      <c r="A3" s="60"/>
+      <c r="B3" s="62" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="60"/>
+    </row>
+    <row r="4" spans="1:8" ht="9" customHeight="1">
+      <c r="A4" s="60"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="60"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="60"/>
+      <c r="B5" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="60"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="60"/>
+      <c r="B6" s="60" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="60"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="60"/>
+      <c r="B7" s="60" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="60"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="60"/>
+      <c r="B8" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="60"/>
+    </row>
+    <row r="9" spans="1:8" ht="6" customHeight="1"/>
+    <row r="10" spans="1:8" ht="69.599999999999994">
+      <c r="B10" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1">
+      <c r="B11" s="65">
+        <v>1</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="68" t="s">
+        <v>245</v>
+      </c>
+      <c r="F11" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1">
+      <c r="B12" s="65">
+        <v>2</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" s="71" t="s">
+        <v>248</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>260</v>
+      </c>
+      <c r="G12" s="71" t="s">
+        <v>249</v>
+      </c>
+      <c r="H12" s="72" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" customHeight="1"/>
+  </sheetData>
+  <autoFilter ref="B10:H12"/>
+  <phoneticPr fontId="1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.35433070866141736" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="76" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;P／&amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>